<commit_message>
Substituição do JUnit pelo TestNG
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java-codigo\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5629168-EA47-4572-A78C-6F2B440BC453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D7F084-28A4-4F90-B82A-0BE1D39F7BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Oicara10</t>
   </si>
@@ -94,9 +94,6 @@
     <t>PostalCode:</t>
   </si>
   <si>
-    <t>User name already exists</t>
-  </si>
-  <si>
     <t>Username field is required</t>
   </si>
   <si>
@@ -169,7 +166,19 @@
     <t>No results for "Guitarra"</t>
   </si>
   <si>
-    <t>john11</t>
+    <t>Quantidade:</t>
+  </si>
+  <si>
+    <t>Oops! We only have 10 in stock. We updated your order accordingly</t>
+  </si>
+  <si>
+    <t>Dados cadastrais</t>
+  </si>
+  <si>
+    <t>Asserts campos obrigatório</t>
+  </si>
+  <si>
+    <t>john147</t>
   </si>
 </sst>
 </file>
@@ -249,12 +258,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -297,12 +306,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -312,6 +356,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -599,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +662,7 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
@@ -623,150 +675,139 @@
     <col min="16" max="16" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="D1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="3" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>25</v>
+      <c r="B14" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D02004DB-1210-4383-AD1F-180E7A556195}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{BD8F867D-A7BF-4942-BF05-BC0B763D904B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -775,107 +816,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14751EE3-3E98-47B5-9840-2A22BE6B35CE}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -883,5 +936,6 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementação do report dos casos de testes
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java-codigo\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D7F084-28A4-4F90-B82A-0BE1D39F7BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C71AA8-A94C-453F-B9D3-80E65326DFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Oicara10</t>
   </si>
@@ -178,7 +178,10 @@
     <t>Asserts campos obrigatório</t>
   </si>
   <si>
-    <t>john147</t>
+    <t>john1475</t>
+  </si>
+  <si>
+    <t>999</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -358,6 +361,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,6 +373,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -653,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,10 +683,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
       <c r="D1" s="10" t="s">
         <v>49</v>
       </c>
@@ -692,6 +699,7 @@
       <c r="B2" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
@@ -818,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14751EE3-3E98-47B5-9840-2A22BE6B35CE}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,18 +894,18 @@
       <c r="C5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="3">
-        <v>999</v>
+      <c r="D5" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">

</xml_diff>

<commit_message>
Implementado algumas documentações e refatoração
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java-codigo\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B63C68-1455-4117-8068-74955F4F88A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1C1137-B32C-4F69-9AA1-4847DA2B9C31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Oicara10</t>
   </si>
@@ -178,13 +178,10 @@
     <t>Asserts campos obrigatório</t>
   </si>
   <si>
-    <t>john1475</t>
-  </si>
-  <si>
     <t>999</t>
   </si>
   <si>
-    <t>john120</t>
+    <t>john1229</t>
   </si>
 </sst>
 </file>
@@ -700,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="3" t="s">
@@ -809,7 +806,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -830,7 +827,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +895,7 @@
         <v>47</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refatoração dos metodos de busca do selenium
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java-codigo\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ws-eclipse-projetoAvaliacaoRSI\automacao-treinamentoHub-TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1C1137-B32C-4F69-9AA1-4847DA2B9C31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
     <sheet name="Produtos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,13 +180,13 @@
     <t>999</t>
   </si>
   <si>
-    <t>john1229</t>
+    <t>john117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -657,7 +656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -815,7 +814,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{BD8F867D-A7BF-4942-BF05-BC0B763D904B}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -823,7 +822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14751EE3-3E98-47B5-9840-2A22BE6B35CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Refatoração na estrutura pageFactory
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -180,7 +180,7 @@
     <t>999</t>
   </si>
   <si>
-    <t>john117</t>
+    <t>john1115</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Algumas melhorias no código e estrutura
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ws-eclipse-projetoAvaliacaoRSI\automacao-treinamentoHub-TDD\target\dadosParaTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Selenium_Automacao\ProjectTreinamentoHub-TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C78D2FA-8054-4D37-8728-5135D3A3B86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -180,13 +181,13 @@
     <t>999</t>
   </si>
   <si>
-    <t>john1115</t>
+    <t>john1116</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -656,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +815,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -822,7 +823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Implementado Suite de Testes
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA783B42-DE48-410D-A04B-D2554F2FDB33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F9A23-0444-457D-8FC2-D5D9CFF327CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <t>999</t>
   </si>
   <si>
-    <t>john1106</t>
+    <t>john1126</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Foi implementado a classe responsavel pelo armazenamento dos dados do excel
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F9A23-0444-457D-8FC2-D5D9CFF327CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA42A946-D1F7-4CF7-B490-025DC385B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <t>999</t>
   </si>
   <si>
-    <t>john1126</t>
+    <t>john1129</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Melhorando o status report
</commit_message>
<xml_diff>
--- a/target/dadosParaTest/massaDeDadosTestes.XLSX
+++ b/target/dadosParaTest/massaDeDadosTestes.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\dadosParaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA42A946-D1F7-4CF7-B490-025DC385B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D09CED3-3D35-4E24-A3DA-918C359F4A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -181,7 +181,7 @@
     <t>999</t>
   </si>
   <si>
-    <t>john1129</t>
+    <t>johnata10</t>
   </si>
 </sst>
 </file>

</xml_diff>